<commit_message>
added auction budget prediction code, updated draft app
</commit_message>
<xml_diff>
--- a/Fantasy Draft.xlsx
+++ b/Fantasy Draft.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="220" windowWidth="23000" windowHeight="9860"/>
+    <workbookView xWindow="480" yWindow="220" windowWidth="23000" windowHeight="15700"/>
   </bookViews>
   <sheets>
     <sheet name="Drafted" sheetId="1" r:id="rId1"/>
@@ -1320,10 +1320,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1820,8 +1820,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1841,7 +1841,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1853,7 +1853,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1865,7 +1865,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2060,7 +2060,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2069,7 +2069,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2400,7 +2400,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>